<commit_message>
retrieving misconception from LLM
</commit_message>
<xml_diff>
--- a/OLI_TransactionData_Analyze/sorted_data/Betsune/Betsune_sorted_by_av_inputlen_Multi_Steps.xlsx
+++ b/OLI_TransactionData_Analyze/sorted_data/Betsune/Betsune_sorted_by_av_inputlen_Multi_Steps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/machi/Desktop/OLI_TransactionData_Analyze/sorted_data/Betsune/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/machi/Documents/GitHub/Misconception_Analysis/OLI_TransactionData_Analyze/sorted_data/Betsune/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42650C75-F0AA-6744-84A3-841645286BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C038F74-EE9A-624A-9F38-834CE4D20135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{04992744-F79F-3D42-884B-FC5E74B8A3F5}"/>
+    <workbookView xWindow="1480" yWindow="1300" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{04992744-F79F-3D42-884B-FC5E74B8A3F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="116" r:id="rId3"/>
+    <pivotCache cacheId="179" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -11226,7 +11226,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CC0C404F-866A-B840-BCD5-C5325B09C847}" name="PivotTable17" cacheId="116" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CC0C404F-866A-B840-BCD5-C5325B09C847}" name="PivotTable17" cacheId="179" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:D24" firstHeaderRow="1" firstDataRow="1" firstDataCol="4"/>
   <pivotFields count="11">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -11890,7 +11890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05CF8A1-C686-EF48-B354-D07D131F4CA1}">
   <dimension ref="A3:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -12179,11 +12179,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96285105-BC18-5540-9B89-AB6707CAEC20}">
   <dimension ref="A1:K676"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="11" width="25" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" customWidth="1"/>
+    <col min="4" max="11" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>